<commit_message>
removed spark context log
</commit_message>
<xml_diff>
--- a/files_prod/master_specs.xlsx
+++ b/files_prod/master_specs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hando\dev\standard-data-management-framework\files_prod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hando\dev2\sdmf-official\files_prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545E6D85-0D9B-4015-8F2E-B8BE5CAD0CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7460B-D49A-4BDE-9673-433246439884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="209" xr2:uid="{9E3D2F59-A0F5-48A1-B731-1D8811F4785E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>feed_id</t>
   </si>
@@ -185,218 +185,22 @@
     <t>bronze</t>
   </si>
   <si>
-    <t>LANGUAGE</t>
-  </si>
-  <si>
-    <t>iso_language_codes</t>
-  </si>
-  <si>
-    <t>t_iso_language_codes</t>
-  </si>
-  <si>
-    <t>{
-    "vacuum_hours": 168,
-    "partition_keys": [],
-    "selection_schema": {
-        "type": "struct",
-        "fields": [
-            {
-                "name": "official_lang_code",
-                "type": "string",
-                "nullable": false,
-                "metadata": {}
-            },
-            {
-                "name": "iso2_code",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "iso3_code",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "onu_code",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "is_ilomember",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "is_receiving_quest",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "label_en",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "label_fr",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "label_sp",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "geo_shape",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            },
-            {
-                "name": "geo_point_2d",
-                "type": "string",
-                "nullable": true,
-                "metadata": {}
-            }
-        ]
-    },
-    "ingestion_config": {
-        "request": {
-            "url": "https://hub.huwise.com/api/explore/v2.1/catalog/datasets/countries-codes/exports/parquet/",
-            "method": "GET",
-            "headers": {},
-            "params": {
-                "lang": "en",
-                "timezone": "Asia/Calcutta"
-            },
-            "body": null,
-            "timeout": 30
-        },
-        "response": {
-            "format": "parquet",
-            "content_type": "application/parquet",
-            "compression": "none",
-            "file_layout": "single",
-            "infer_schema": true
-        },
-        "retry": {
-            "enabled": true,
-            "max_attempts": 3,
-            "backoff_factor": 2.0,
-            "max_backoff": 30,
-            "retry_statuses": [
-                429,
-                500,
-                502,
-                503,
-                504
-            ]
-        },
-        "deduplication": {
-            "enabled": false
-        },
-        "metadata": {
-            "source": "huwise",
-            "feed_type": "api",
-            "owner": "data-platform",
-            "sla": "daily"
-        }
-    }
-}</t>
-  </si>
-  <si>
     <t>API_EXTRACTOR</t>
   </si>
   <si>
-    <t>yalsworld_datawarehouse</t>
-  </si>
-  <si>
     <t>SOURCE_TO_BRONZE</t>
   </si>
   <si>
-    <t>BRONZE</t>
-  </si>
-  <si>
     <t>SOURCE</t>
   </si>
   <si>
     <t>iso_language_codes_raw</t>
   </si>
   <si>
-    <t>country_codes_raw</t>
-  </si>
-  <si>
-    <t>DELTA_TABLE</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
     <t>t_iso_language_codes_raw</t>
   </si>
   <si>
-    <t>t_country_codes_raw</t>
-  </si>
-  <si>
-    <t>{
-    "primary_key": "alpha3_b",
-    "composite_key": [],
-    "partition_keys": [],
-    "vacuum_hours": 168,
-    "source_table_name": "yalsworld_datawarehouse.bronze.t_iso_language_codes",
-    "selection_query":null,
-    "selection_schema": {
-        "type": "struct",
-        "fields": [
-            {
-                "name": "alpha3_b",
-                "type": "string",
-                "nullable": true
-            },
-            {
-                "name": "alpha3_t",
-                "type": "string",
-                "nullable": true
-            },
-            {
-                "name": "alpha2",
-                "type": "string",
-                "nullable": true
-            },
-            {
-                "name": "english",
-                "type": "string",
-                "nullable": true
-            }
-        ]
-    },
-    "standard_checks": [
-        {
-            "check_sequence": [
-                "_check_primary_key"
-            ],
-            "column_name": "alpha3_b",
-            "threshold": 0
-        },
-        {
-            "check_sequence": [
-                "_check_nulls"
-            ],
-            "column_name": "english",
-            "threshold": 0
-        }
-    ],
-    "comprehensive_checks": [
-    ]
-}</t>
+    <t>sdmf</t>
   </si>
 </sst>
 </file>
@@ -494,8 +298,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{607A0EF2-7813-403A-A324-C8BA6E6AB114}" name="master_specs" displayName="master_specs" ref="A1:R4" totalsRowShown="0">
-  <autoFilter ref="A1:R4" xr:uid="{607A0EF2-7813-403A-A324-C8BA6E6AB114}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{607A0EF2-7813-403A-A324-C8BA6E6AB114}" name="master_specs" displayName="master_specs" ref="A1:R2" totalsRowShown="0">
+  <autoFilter ref="A1:R2" xr:uid="{607A0EF2-7813-403A-A324-C8BA6E6AB114}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{79DEFD1E-C4B7-4717-97F6-0D39BE9CE126}" name="feed_id"/>
     <tableColumn id="2" xr3:uid="{590CECDE-6BE1-49B1-8A26-5436C9A95313}" name="system_name"/>
@@ -819,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A6F937-D7CE-4353-901E-FC6AEF049B39}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,13 +724,13 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
         <v>23</v>
@@ -935,7 +739,7 @@
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -944,7 +748,7 @@
         <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="O2" t="str">
         <f t="shared" ref="O2" si="0">_xlfn.CONCAT("t_uid_",A2,"_",LEFT(B2, 1), LEFT(C2, 1), LEFT(D2, 1), LEFT(E2, 1), LEFT(I2, 1), "_", K2,"_",H2)</f>
@@ -960,176 +764,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" t="str">
-        <f>_xlfn.CONCAT("t_uid_",A3,"_",LEFT(B3, 1), LEFT(C3, 1), LEFT(D3, 1), LEFT(E3, 1), LEFT(I3, 1), "_", K3,"_",H3)</f>
-        <v>t_uid_2_YGCLP_API_EXTRACTOR_country_codes_raw</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" t="str">
-        <f>_xlfn.CONCAT("t_uid_",A4,"_",LEFT(B4, 1), LEFT(C4, 1), LEFT(D4, 1), LEFT(E4, 1), LEFT(I4, 1), "_", K4,"_",H4)</f>
-        <v>t_uid_3_YGCCD_API_EXTRACTOR_iso_language_codes</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A4">
-    <cfRule type="cellIs" dxfId="4" priority="32" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="3" priority="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:R4">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+  <conditionalFormatting sqref="A2:R2">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
-    <cfRule type="duplicateValues" dxfId="1" priority="34"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="cellIs" dxfId="3" priority="36" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="2" priority="37"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N4">
-    <cfRule type="duplicateValues" dxfId="0" priority="35"/>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="duplicateValues" dxfId="1" priority="38"/>
   </conditionalFormatting>
-  <dataValidations count="14">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{7E208DA3-F201-4D55-8871-75223992D6F6}">
+  <conditionalFormatting sqref="N2">
+    <cfRule type="duplicateValues" dxfId="0" priority="39"/>
+  </conditionalFormatting>
+  <dataValidations count="13">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7E208DA3-F201-4D55-8871-75223992D6F6}">
       <formula1>"YALS_WORLD"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{0B03C047-76E9-42CB-AC60-57D9606D2481}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0B03C047-76E9-42CB-AC60-57D9606D2481}">
       <formula1>"DATA_ENRICHMENT,GENERIC"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{483113FD-1194-4C33-99BA-0094FA37F1CA}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{483113FD-1194-4C33-99BA-0094FA37F1CA}">
       <formula1>"CODES,RELIGION"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{DD60934B-F5B2-4013-9719-3135E2D233D1}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{DD60934B-F5B2-4013-9719-3135E2D233D1}">
       <formula1>"COUNTRY,LANGUAGE,HINDUISM,ISLAM,CHRISTIANITY"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{D5871B94-C844-4AC3-BC5A-D1C89244F32D}">
-      <formula1>"DELTA_TABLE,JSON,CSV,PARQUET,XLSX"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID TARGET TABLE NAME" error="Please read the feed name rules by clicking on the feed_name data cell. Non-Compliance to feed name rules is strictly prohibited. Even if excel validation is successful, SDMF may not process feeds if rules are invalidated." promptTitle="Target Table Name Rules" prompt="1.No leading or trailing spaces_x000a_2.No spaces inside the text_x000a_3.All lowercase letters_x000a_4.Does not start with a number_x000a_5.Length is at least 3 characters_x000a_6.Length is no more than 50 characters_x000a_7.Text must start with &quot;t_&quot;_x000a_DO NOT INCLUDE SPECIAL CHARACTERS" sqref="N2:N4" xr:uid="{4FAD78C1-A717-46A8-8B62-E0E28A665134}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{D5871B94-C844-4AC3-BC5A-D1C89244F32D}">
+      <formula1>"DELTA_TABLE,JSON,CSV,PARQUET,XLSX,XML"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID TARGET TABLE NAME" error="Please read the feed name rules by clicking on the feed_name data cell. Non-Compliance to feed name rules is strictly prohibited. Even if excel validation is successful, SDMF may not process feeds if rules are invalidated." promptTitle="Target Table Name Rules" prompt="1.No leading or trailing spaces_x000a_2.No spaces inside the text_x000a_3.All lowercase letters_x000a_4.Does not start with a number_x000a_5.Length is at least 3 characters_x000a_6.Length is no more than 50 characters_x000a_7.Text must start with &quot;t_&quot;_x000a_DO NOT INCLUDE SPECIAL CHARACTERS" sqref="N2" xr:uid="{4FAD78C1-A717-46A8-8B62-E0E28A665134}">
       <formula1>AND(N2&lt;&gt;"",N2=TRIM(N2),ISERROR(SEARCH(" ",N2)),N2=LOWER(N2),NOT(ISNUMBER(--LEFT(N2,1))),LEN(N2)&gt;=3,LEN(N2)&lt;=50,LEFT(N2,2)="t_")</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="H2:H4 J2:J4" xr:uid="{43A1729D-1187-4114-BCC7-69F23DF7B2DF}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{6ACEFD19-F3D1-4074-A1E0-3114AC5C3633}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="H2 J2" xr:uid="{43A1729D-1187-4114-BCC7-69F23DF7B2DF}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{6ACEFD19-F3D1-4074-A1E0-3114AC5C3633}">
       <formula1>"EXTRACTION,SOURCE_TO_BRONZE,BRONZE_TO_SILVER,SILVER_TO_GOLD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G4" xr:uid="{5825120F-D012-47BA-B828-E28B3B293C20}">
-      <formula1>"EXTERNAL,SOURCE,BRONZE,SILVER,GOLD"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R4" xr:uid="{D889056B-B881-4521-861C-659903490942}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{D889056B-B881-4521-861C-659903490942}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2:L4" xr:uid="{25792A68-0714-4780-856C-C89C05C858D7}">
-      <formula1>"testing,yalsworld_datawarehouse"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2:M4" xr:uid="{8DE01F92-A7E3-4904-AFF6-21122520A11C}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{25792A68-0714-4780-856C-C89C05C858D7}">
+      <formula1>"testing,sdmf"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{8DE01F92-A7E3-4904-AFF6-21122520A11C}">
       <formula1>"bronze,silver,gold"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K2:K4" xr:uid="{B2C7DA7D-8D0C-4838-AF83-029786900D6A}">
-      <formula1>"FULL_LOAD,APPEND_LOAD,INCREMENTAL_CDC,SCD_TYPE_2,API_EXTRACTOR"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{B2C7DA7D-8D0C-4838-AF83-029786900D6A}">
+      <formula1>"FULL_LOAD,APPEND_LOAD,INCREMENTAL_CDC,SCD_TYPE_2,API_EXTRACTOR,STORAGE_FETCH"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{B4488FCE-160F-4AFB-8EC5-F9C5095A62C9}">
       <formula1>"SOURCE,BRONZE,SILVER,GOLD"</formula1>

</xml_diff>